<commit_message>
add prabowo data CV
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="386">
   <si>
     <t>GET /v1/president/{electionNumber}</t>
   </si>
@@ -224,6 +224,9 @@
     <t>Ir. H. Joko Widodo</t>
   </si>
   <si>
+    <t>Prabowo Subianto</t>
+  </si>
+  <si>
     <t>nik</t>
   </si>
   <si>
@@ -251,18 +254,27 @@
     <t>Jalam Medan Merdeka Utara RT.05 RW 02. Kecamatan Gambir, Kota Jakarta Pusat, DKI Jakarta</t>
   </si>
   <si>
+    <t>Kp Gombong RT. 03, RW 09 Kelurahan Bojong Koneng, Kecamatan Babakan Madang, Kabupaten Bogor, Jawa Barat</t>
+  </si>
+  <si>
     <t>maritalStatus</t>
   </si>
   <si>
     <t>Kawin</t>
   </si>
   <si>
+    <t>Cerai Hidup</t>
+  </si>
+  <si>
     <t>wifeName</t>
   </si>
   <si>
     <t>Hj. Iriana, S.E., M.M</t>
   </si>
   <si>
+    <t>Siti Hediati Haryadi</t>
+  </si>
+  <si>
     <t>childrenCount</t>
   </si>
   <si>
@@ -272,12 +284,18 @@
     <t>Strata-1 (S1)</t>
   </si>
   <si>
+    <t>Akademi Militer Nasional</t>
+  </si>
+  <si>
     <t>occupation</t>
   </si>
   <si>
     <t>Presiden Republik Indonesia</t>
   </si>
   <si>
+    <t>Purnawirawan TNI / Pengusaha</t>
+  </si>
+  <si>
     <t>education</t>
   </si>
   <si>
@@ -287,84 +305,153 @@
     <t>Sarjana Strata 1 (S1)</t>
   </si>
   <si>
+    <t>TK</t>
+  </si>
+  <si>
     <t>place</t>
   </si>
   <si>
     <t>Universitas Gadjah Mada (UGM) - Fakultas Kehutanan</t>
   </si>
   <si>
+    <t>Sekolah Sumbangsih, Jakarta, Indonesia</t>
+  </si>
+  <si>
     <t>fromToYear</t>
   </si>
   <si>
     <t>1980-1985</t>
   </si>
   <si>
+    <t>1956-1957</t>
+  </si>
+  <si>
     <t>Sekolah Menengah Atas</t>
   </si>
   <si>
+    <t>SD</t>
+  </si>
+  <si>
     <t>SMA Negri 6 Solo</t>
   </si>
   <si>
+    <t>The Dean School, Singapura</t>
+  </si>
+  <si>
     <t>1976-1980</t>
   </si>
   <si>
+    <t>1957-1960</t>
+  </si>
+  <si>
     <t>Sekolah Menengah Pertama</t>
   </si>
   <si>
+    <t>Glenealy Junior School, Hongkong</t>
+  </si>
+  <si>
     <t>SMP Negri 1 Solo</t>
   </si>
   <si>
+    <t>1960-1962</t>
+  </si>
+  <si>
     <t>1973-1976</t>
   </si>
   <si>
+    <t>SMP</t>
+  </si>
+  <si>
     <t>Sekolah Dasar</t>
   </si>
   <si>
+    <t>Victoria Institute, Kuala Lumpur, Malaysia</t>
+  </si>
+  <si>
     <t>SDN 111 Tirtoyoso</t>
   </si>
   <si>
+    <t>1962-1964</t>
+  </si>
+  <si>
     <t>1967-1973</t>
   </si>
   <si>
     <t>organization</t>
   </si>
   <si>
+    <t>American International School</t>
+  </si>
+  <si>
     <t>ASMINDO Komda Surakarta</t>
   </si>
   <si>
+    <t>1964-1966</t>
+  </si>
+  <si>
     <t>position</t>
   </si>
   <si>
     <t>Ketua</t>
   </si>
   <si>
+    <t>SMA</t>
+  </si>
+  <si>
     <t>2002-2007</t>
   </si>
   <si>
+    <t>The American School in London</t>
+  </si>
+  <si>
     <t>Kadin Surakarta</t>
   </si>
   <si>
+    <t>1966-1968</t>
+  </si>
+  <si>
     <t>Ketua Bidang Pertambangan dan Energi</t>
   </si>
   <si>
+    <t>Akademi Militer Nasional, Magelang Indonesia</t>
+  </si>
+  <si>
     <t>1992-1996</t>
   </si>
   <si>
+    <t>1970-1974</t>
+  </si>
+  <si>
     <t>jobExperience</t>
   </si>
   <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>German GSG-9 anti-terror</t>
+  </si>
+  <si>
     <t>Gubernur DKI Jakarta</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
     <t>2012-2014</t>
   </si>
   <si>
+    <t>Fort Benning</t>
+  </si>
+  <si>
     <t>Walikota Surakarta</t>
   </si>
   <si>
     <t>2010-2012</t>
   </si>
   <si>
+    <t>Yayasan Pendidikan Kebangsaan</t>
+  </si>
+  <si>
     <t>2005-2010</t>
   </si>
   <si>
@@ -374,6 +461,9 @@
     <t>-</t>
   </si>
   <si>
+    <t>Himpunan Kerukunan Tani Indonesia (HKTI)</t>
+  </si>
+  <si>
     <t>jobAppreciation</t>
   </si>
   <si>
@@ -386,27 +476,42 @@
     <t>The Royal Islamic Strategic Studies Center, Jordan</t>
   </si>
   <si>
-    <t>year</t>
+    <t>Partai Gerindra</t>
   </si>
   <si>
     <t>Man of The Year</t>
   </si>
   <si>
+    <t>Ketua Umum dan Ketua Dewan Pembina</t>
+  </si>
+  <si>
     <t>Globe Asia Magazine</t>
   </si>
   <si>
+    <t>Ikatan Pencak Silat Indonesia</t>
+  </si>
+  <si>
     <t>Global Islamic Finance Leadership Award</t>
   </si>
   <si>
+    <t>Ketua Umum</t>
+  </si>
+  <si>
     <t>Edbiz Consulting - Shari'a Advisory Firm</t>
   </si>
   <si>
+    <t>Asosiasi Pedagang Pasar Seluruh Indonesia</t>
+  </si>
+  <si>
     <t>The 100 Most Influential People</t>
   </si>
   <si>
     <t>Time Magazine</t>
   </si>
   <si>
+    <t>Koperasi Garuda Yaksa</t>
+  </si>
+  <si>
     <t>The World's 50 Greatest Leader</t>
   </si>
   <si>
@@ -416,123 +521,195 @@
     <t>Antara Achievement Award</t>
   </si>
   <si>
+    <t>TNI - Komandan Jendral Kopassus</t>
+  </si>
+  <si>
     <t>Kantor Berita Antara</t>
   </si>
   <si>
+    <t>1996-1998</t>
+  </si>
+  <si>
+    <t>TNI - Panglima Komando Cadangan Strategis Angkatan Darat</t>
+  </si>
+  <si>
     <t>Anugerah Pangripta Nusantara Pratama (Tingkat Provinsi - Kelompok A) Pencapaian Tujuan Pembangunan Melenium</t>
   </si>
   <si>
+    <t>1998-1998</t>
+  </si>
+  <si>
     <t>Bappenas RI</t>
   </si>
   <si>
+    <t>TNI - Komandan Sekolah Staf dan Komando ABRI</t>
+  </si>
+  <si>
     <t>Democracy Award 2013</t>
   </si>
   <si>
+    <t>PT Nusantara Energy - Presiden Direktur</t>
+  </si>
+  <si>
     <t>RMOL</t>
   </si>
   <si>
+    <t>PT Kertas Nusantara - Presiden Direktur</t>
+  </si>
+  <si>
     <t>Award on Good Government, Kategori Kepemerintahan Terbaik</t>
   </si>
   <si>
+    <t>2001-2009</t>
+  </si>
+  <si>
     <t>Soegeng Sarjadi School ot Government</t>
   </si>
   <si>
+    <t>PT Tidar Kerinci Agung - Komisaris Utama</t>
+  </si>
+  <si>
     <t>Word Mayor Project (Third Place)</t>
   </si>
   <si>
+    <t>Bintang kartika Eka Paksi Nararya</t>
+  </si>
+  <si>
     <t>The City Mayors Foundation</t>
   </si>
   <si>
     <t>Green City - Surakarta</t>
   </si>
   <si>
+    <t>Satya Lencana Kesetiaan XVI Tahun</t>
+  </si>
+  <si>
     <t>The La Tofi School of CSR</t>
   </si>
   <si>
     <t>Kategiru Kotamadya - Walikota Terbaik</t>
   </si>
   <si>
+    <t>Satya Lencana Seroja Ulangan-III</t>
+  </si>
+  <si>
     <t>Majalah GATRA</t>
   </si>
   <si>
     <t>Bintang Jasa Utama</t>
   </si>
   <si>
+    <t>Satya Lencana Raksaka Dharma</t>
+  </si>
+  <si>
     <t>Presiden RI</t>
   </si>
   <si>
     <t>Satyalencana Pembangunan Bidang Koperasi</t>
   </si>
   <si>
+    <t>Satya Lencana Dwija Sistha</t>
+  </si>
+  <si>
     <t>Tokoh Perubahan 2010</t>
   </si>
   <si>
+    <t>Satya Lencana Wira Karya</t>
+  </si>
+  <si>
     <t>Republika</t>
   </si>
   <si>
     <t>Dharma Bakti Praja</t>
   </si>
   <si>
+    <t>The First Class The Padin Medal Ops Honor</t>
+  </si>
+  <si>
     <t>UNS</t>
   </si>
   <si>
+    <t>Pemerintah Kamboja</t>
+  </si>
+  <si>
     <t>Bung Hatta Anti Corruption Award</t>
   </si>
   <si>
+    <t>Bintang Yudha Dharma Nararya</t>
+  </si>
+  <si>
     <t>Perkumpulan Bung Hatta Anti-Corruption Award</t>
   </si>
   <si>
     <t>Innovative Government Award - Kategori Pelayanan Publik</t>
   </si>
   <si>
+    <t>publication</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
     <t>Kemendagri RI</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Selamatkan Indonesia Raya</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>Alumni Awards Bidang Penggerak Sosial</t>
   </si>
   <si>
+    <t>Membangun Kembali Indonesia Raya</t>
+  </si>
+  <si>
     <t>UGM</t>
   </si>
   <si>
+    <t>Paradok Indonesia</t>
+  </si>
+  <si>
     <t>Tokoh TEMPO 2008</t>
   </si>
   <si>
     <t>Majalah TEMPO</t>
   </si>
   <si>
-    <t>publication</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
-    <t>title</t>
+    <t>motivation</t>
+  </si>
+  <si>
+    <t>(berisi hal-hal yang melatarbelakangi calon untuk mengajukan diri sebagai bakal calon Presiden dan Wakil Presiden)</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>(berisi contoh hal-hal yang akan dikerjakan ketika telah menjadi Presiden dan Wakil Presiden)</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>https://kpu.go.id/koleksigambar/BB.2_PPWP_2.pdf</t>
   </si>
   <si>
     <t>"Revolusi Mental", Opini KOMPAS</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>10-Mei-2014</t>
   </si>
   <si>
-    <t>motivation</t>
-  </si>
-  <si>
     <t>Melanjutkan dan menyesaikan kerja nyata yang dimulai sejak Oktober 2014 untuk Indonesia yang sejahtera dan berkeadilan.</t>
   </si>
   <si>
-    <t>target</t>
-  </si>
-  <si>
     <t>Transformasi manusia Indonesia yang maju, unggul dan sejahtera. Transformasi menuju struktur ekonomi produktif, mandiri dan berdaya saing. Transformasi menuju pembangunan yang merata dan berkeadilan. Transformasi kebudayaan menuju kepribadian bangsa yang berakhlak mulia dan berbhinneka tunggal ika. Transformasi menuju pembangunan lingkungan hidup yang berkelanjutan</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>https://kpu.go.id/koleksigambar/BB.2_PPWP_.pdf</t>
   </si>
   <si>
@@ -596,9 +773,6 @@
     <t>MUI</t>
   </si>
   <si>
-    <t>Ketua Umum</t>
-  </si>
-  <si>
     <t>Watimpres</t>
   </si>
   <si>
@@ -744,9 +918,6 @@
   </si>
   <si>
     <t>Ketua Front Pemuda</t>
-  </si>
-  <si>
-    <t>1964-1966</t>
   </si>
   <si>
     <t>PC GP Ansor Tanjung Priuk</t>
@@ -1539,6 +1710,9 @@
       <c r="B29" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="E29" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
@@ -1547,221 +1721,389 @@
       <c r="C30" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="E30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>69</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>3174031710510000</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>22453</v>
       </c>
+      <c r="E32" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>18918</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>72</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>74</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>76</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E38" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="E41" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>93</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D48" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F48" s="0" t="s">
         <v>96</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>97</v>
+        <v>110</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>99</v>
+        <v>114</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="F54" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>103</v>
+        <v>121</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>105</v>
+        <v>124</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>106</v>
+        <v>126</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,47 +2111,86 @@
         <v>4</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>107</v>
+        <v>128</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>108</v>
+        <v>130</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>109</v>
+        <v>132</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="E61" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>111</v>
+        <v>137</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>1981</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>112</v>
+        <v>139</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,15 +2198,27 @@
         <v>4</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>113</v>
+        <v>141</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>1985</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>114</v>
+        <v>142</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,15 +2226,27 @@
         <v>4</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>113</v>
+        <v>141</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>115</v>
+        <v>144</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,546 +2254,928 @@
         <v>4</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>116</v>
+        <v>145</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>2001</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>117</v>
+        <v>146</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>119</v>
+        <v>149</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>121</v>
+        <v>151</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>2004</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>2018</v>
       </c>
+      <c r="F72" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D73" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F73" s="0" t="s">
         <v>123</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>124</v>
+        <v>155</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>2008</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>2016</v>
       </c>
+      <c r="F75" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>125</v>
+        <v>157</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>126</v>
+        <v>159</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>2004</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>2016</v>
       </c>
+      <c r="F78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>127</v>
+        <v>161</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>128</v>
+        <v>162</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>2015</v>
       </c>
+      <c r="F81" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>129</v>
+        <v>164</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>130</v>
+        <v>165</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>2015</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>2014</v>
       </c>
+      <c r="E84" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>131</v>
+        <v>166</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>132</v>
+        <v>168</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>2014</v>
       </c>
+      <c r="F87" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>133</v>
+        <v>171</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>134</v>
+        <v>173</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>2013</v>
       </c>
+      <c r="F90" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>135</v>
+        <v>175</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>136</v>
+        <v>177</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <v>2002</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>2013</v>
       </c>
+      <c r="F93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>137</v>
+        <v>179</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>138</v>
+        <v>181</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D96" s="0" t="n">
         <v>2012</v>
       </c>
+      <c r="F96" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G96" s="0" t="n">
+        <v>2002</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>139</v>
+        <v>183</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>140</v>
+        <v>185</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>2012</v>
       </c>
+      <c r="F99" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>141</v>
+        <v>186</v>
+      </c>
+      <c r="E100" s="7"/>
+      <c r="F100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>142</v>
+        <v>188</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>2012</v>
       </c>
+      <c r="F102" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G102" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>143</v>
+        <v>189</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G103" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>144</v>
+        <v>191</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>2011</v>
       </c>
+      <c r="F105" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>145</v>
+        <v>192</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D107" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G107" s="0" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>3022</v>
       </c>
+      <c r="F108" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>147</v>
+        <v>195</v>
+      </c>
+      <c r="F109" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D110" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="F110" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G110" s="0" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D111" s="0" t="n">
         <v>2011</v>
       </c>
+      <c r="F111" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G111" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>148</v>
+        <v>197</v>
+      </c>
+      <c r="F112" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G112" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>149</v>
+        <v>199</v>
+      </c>
+      <c r="F113" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G113" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D114" s="0" t="n">
         <v>2011</v>
       </c>
+      <c r="F114" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G114" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>150</v>
+        <v>200</v>
+      </c>
+      <c r="F115" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G115" s="0" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>151</v>
+        <v>202</v>
+      </c>
+      <c r="F116" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G116" s="0" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D117" s="0" t="n">
         <v>2011</v>
       </c>
+      <c r="F117" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>152</v>
+        <v>204</v>
+      </c>
+      <c r="F118" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G118" s="0" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>153</v>
+        <v>206</v>
+      </c>
+      <c r="F119" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D120" s="0" t="n">
         <v>2010</v>
       </c>
+      <c r="F120" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>154</v>
+        <v>207</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F121" s="0" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>155</v>
+        <v>210</v>
+      </c>
+      <c r="F122" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="G122" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D123" s="0" t="n">
         <v>2010</v>
       </c>
+      <c r="F123" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="G123" s="0" t="n">
+        <v>2009</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>156</v>
+        <v>214</v>
+      </c>
+      <c r="F124" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="G124" s="0" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>157</v>
+        <v>216</v>
+      </c>
+      <c r="F125" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="G125" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>2010</v>
       </c>
+      <c r="F126" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="G126" s="0" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>158</v>
+        <v>218</v>
+      </c>
+      <c r="F127" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="G127" s="0" t="n">
+        <v>2015</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>159</v>
+        <v>219</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="F128" s="0" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D129" s="0" t="n">
         <v>2008</v>
       </c>
+      <c r="E129" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="F129" s="0" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="0" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>161</v>
+        <v>209</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F130" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>163</v>
+        <v>226</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>165</v>
+        <v>227</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="0" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>167</v>
+        <v>228</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="0" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="0" t="s">
-        <v>170</v>
+        <v>224</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>171</v>
+        <v>230</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,20 +3183,20 @@
         <v>4</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C139" s="8" t="n">
         <v>15776</v>
@@ -2417,47 +3204,47 @@
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C145" s="0" t="n">
         <v>10</v>
@@ -2465,23 +3252,23 @@
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>17</v>
@@ -2489,125 +3276,125 @@
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>181</v>
+        <v>240</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>182</v>
+        <v>241</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>183</v>
+        <v>242</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>181</v>
+        <v>240</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>184</v>
+        <v>243</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>185</v>
+        <v>244</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>186</v>
+        <v>245</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>187</v>
+        <v>246</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="0" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="C161" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2615,23 +3402,23 @@
         <v>4</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,23 +3426,23 @@
         <v>4</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>194</v>
+        <v>252</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>195</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,23 +3450,23 @@
         <v>4</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>197</v>
+        <v>255</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2687,23 +3474,23 @@
         <v>4</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>198</v>
+        <v>256</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,23 +3498,23 @@
         <v>4</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>200</v>
+        <v>258</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C178" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>202</v>
+        <v>260</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,23 +3522,23 @@
         <v>4</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>203</v>
+        <v>261</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>204</v>
+        <v>262</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>205</v>
+        <v>263</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,23 +3546,23 @@
         <v>4</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>206</v>
+        <v>264</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>207</v>
+        <v>265</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,23 +3570,23 @@
         <v>4</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>208</v>
+        <v>266</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C186" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>209</v>
+        <v>267</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C187" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,23 +3594,23 @@
         <v>4</v>
       </c>
       <c r="D188" s="0" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D189" s="0" t="s">
-        <v>211</v>
+        <v>269</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>212</v>
+        <v>270</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,23 +3618,23 @@
         <v>4</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C192" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>213</v>
+        <v>271</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>214</v>
+        <v>272</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,23 +3642,23 @@
         <v>4</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C195" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>215</v>
+        <v>273</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C196" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>216</v>
+        <v>274</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2879,23 +3666,23 @@
         <v>4</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>217</v>
+        <v>275</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>218</v>
+        <v>276</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C199" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>219</v>
+        <v>277</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,23 +3690,23 @@
         <v>4</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C201" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>221</v>
+        <v>279</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C202" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>219</v>
+        <v>277</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,23 +3714,23 @@
         <v>4</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C204" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>222</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C205" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>223</v>
+        <v>281</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,23 +3738,23 @@
         <v>4</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>224</v>
+        <v>282</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>225</v>
+        <v>283</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2975,23 +3762,23 @@
         <v>4</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>226</v>
+        <v>284</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C210" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>227</v>
+        <v>285</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C211" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>228</v>
+        <v>286</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2999,23 +3786,23 @@
         <v>4</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>229</v>
+        <v>287</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C213" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>230</v>
+        <v>288</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C214" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>231</v>
+        <v>289</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3023,23 +3810,23 @@
         <v>4</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C216" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>233</v>
+        <v>291</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C217" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>234</v>
+        <v>292</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,23 +3834,23 @@
         <v>4</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>235</v>
+        <v>293</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C219" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>236</v>
+        <v>294</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C220" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>234</v>
+        <v>292</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,23 +3858,23 @@
         <v>4</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>237</v>
+        <v>295</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C222" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>238</v>
+        <v>296</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C223" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>239</v>
+        <v>297</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3095,23 +3882,23 @@
         <v>4</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>240</v>
+        <v>298</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C225" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>241</v>
+        <v>299</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C226" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>242</v>
+        <v>122</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3119,23 +3906,23 @@
         <v>4</v>
       </c>
       <c r="D227" s="0" t="s">
-        <v>243</v>
+        <v>300</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C228" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D228" s="0" t="s">
-        <v>244</v>
+        <v>301</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C229" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D229" s="0" t="s">
-        <v>242</v>
+        <v>122</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3143,23 +3930,23 @@
         <v>4</v>
       </c>
       <c r="D230" s="0" t="s">
-        <v>245</v>
+        <v>302</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C231" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D231" s="0" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C232" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D232" s="0" t="s">
-        <v>247</v>
+        <v>304</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,42 +3954,42 @@
         <v>4</v>
       </c>
       <c r="D233" s="0" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C234" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D234" s="0" t="s">
-        <v>249</v>
+        <v>306</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C235" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D235" s="0" t="s">
-        <v>250</v>
+        <v>307</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D236" s="0" t="s">
-        <v>251</v>
+        <v>308</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C237" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D237" s="0" t="s">
-        <v>252</v>
+        <v>309</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,15 +3997,15 @@
         <v>4</v>
       </c>
       <c r="D238" s="0" t="s">
-        <v>253</v>
+        <v>310</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C239" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D239" s="0" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3226,15 +4013,15 @@
         <v>4</v>
       </c>
       <c r="D240" s="0" t="s">
-        <v>254</v>
+        <v>311</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C241" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D241" s="0" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,15 +4029,15 @@
         <v>4</v>
       </c>
       <c r="D242" s="0" t="s">
-        <v>256</v>
+        <v>313</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C243" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D243" s="0" t="s">
-        <v>250</v>
+        <v>307</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,15 +4045,15 @@
         <v>4</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>257</v>
+        <v>314</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C245" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D245" s="0" t="s">
-        <v>250</v>
+        <v>307</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,15 +4061,15 @@
         <v>4</v>
       </c>
       <c r="D246" s="0" t="s">
-        <v>258</v>
+        <v>315</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C247" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D247" s="0" t="s">
-        <v>259</v>
+        <v>316</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3290,15 +4077,15 @@
         <v>4</v>
       </c>
       <c r="D248" s="0" t="s">
-        <v>260</v>
+        <v>317</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C249" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D249" s="0" t="s">
-        <v>250</v>
+        <v>307</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,15 +4093,15 @@
         <v>4</v>
       </c>
       <c r="D250" s="0" t="s">
-        <v>261</v>
+        <v>318</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C251" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D251" s="0" t="s">
-        <v>262</v>
+        <v>319</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,15 +4109,15 @@
         <v>4</v>
       </c>
       <c r="D252" s="0" t="s">
-        <v>263</v>
+        <v>320</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C253" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D253" s="0" t="s">
-        <v>262</v>
+        <v>319</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3338,15 +4125,15 @@
         <v>4</v>
       </c>
       <c r="D254" s="0" t="s">
-        <v>264</v>
+        <v>321</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C255" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D255" s="0" t="s">
-        <v>265</v>
+        <v>322</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,15 +4141,15 @@
         <v>4</v>
       </c>
       <c r="D256" s="0" t="s">
-        <v>266</v>
+        <v>323</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C257" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D257" s="0" t="s">
-        <v>267</v>
+        <v>324</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,15 +4157,15 @@
         <v>4</v>
       </c>
       <c r="D258" s="0" t="s">
-        <v>268</v>
+        <v>325</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C259" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D259" s="0" t="s">
-        <v>269</v>
+        <v>326</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,15 +4173,15 @@
         <v>4</v>
       </c>
       <c r="D260" s="0" t="s">
-        <v>270</v>
+        <v>327</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C261" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D261" s="0" t="s">
-        <v>271</v>
+        <v>328</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,15 +4189,15 @@
         <v>4</v>
       </c>
       <c r="D262" s="0" t="s">
-        <v>272</v>
+        <v>329</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C263" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D263" s="0" t="s">
-        <v>273</v>
+        <v>330</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,39 +4205,39 @@
         <v>4</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>274</v>
+        <v>331</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C265" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D265" s="0" t="s">
-        <v>275</v>
+        <v>332</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="9" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="C266" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D266" s="0" t="s">
-        <v>276</v>
+        <v>333</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C267" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D267" s="0" t="s">
-        <v>277</v>
+        <v>334</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C268" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D268" s="0" t="n">
         <v>2017</v>
@@ -3461,20 +4248,20 @@
         <v>4</v>
       </c>
       <c r="D269" s="0" t="s">
-        <v>278</v>
+        <v>335</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C270" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D270" s="0" t="s">
-        <v>279</v>
+        <v>336</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C271" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D271" s="0" t="n">
         <v>2012</v>
@@ -3485,20 +4272,20 @@
         <v>4</v>
       </c>
       <c r="D272" s="0" t="s">
-        <v>280</v>
+        <v>337</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C273" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D273" s="0" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C274" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D274" s="0" t="n">
         <v>2007</v>
@@ -3509,20 +4296,20 @@
         <v>4</v>
       </c>
       <c r="D275" s="0" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C276" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D276" s="0" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C277" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D277" s="0" t="n">
         <v>2007</v>
@@ -3533,20 +4320,20 @@
         <v>4</v>
       </c>
       <c r="D278" s="0" t="s">
-        <v>282</v>
+        <v>339</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C279" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D279" s="0" t="s">
-        <v>283</v>
+        <v>340</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C280" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D280" s="0" t="n">
         <v>2016</v>
@@ -3557,20 +4344,20 @@
         <v>4</v>
       </c>
       <c r="D281" s="0" t="s">
-        <v>284</v>
+        <v>341</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C282" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D282" s="0" t="s">
-        <v>285</v>
+        <v>342</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C283" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D283" s="0" t="n">
         <v>2018</v>
@@ -3581,20 +4368,20 @@
         <v>4</v>
       </c>
       <c r="D284" s="0" t="s">
-        <v>286</v>
+        <v>343</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C285" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D285" s="0" t="s">
-        <v>287</v>
+        <v>344</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C286" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D286" s="0" t="n">
         <v>2018</v>
@@ -3605,20 +4392,20 @@
         <v>4</v>
       </c>
       <c r="D287" s="0" t="s">
-        <v>288</v>
+        <v>345</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C288" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D288" s="0" t="s">
-        <v>289</v>
+        <v>346</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C289" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D289" s="0" t="n">
         <v>2018</v>
@@ -3629,20 +4416,20 @@
         <v>4</v>
       </c>
       <c r="D290" s="0" t="s">
-        <v>290</v>
+        <v>347</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C291" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>291</v>
+        <v>348</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C292" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D292" s="0" t="n">
         <v>2017</v>
@@ -3653,20 +4440,20 @@
         <v>4</v>
       </c>
       <c r="D293" s="0" t="s">
-        <v>292</v>
+        <v>349</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C294" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D294" s="0" t="s">
-        <v>293</v>
+        <v>350</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C295" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D295" s="0" t="n">
         <v>2017</v>
@@ -3677,20 +4464,20 @@
         <v>4</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>294</v>
+        <v>351</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C297" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>295</v>
+        <v>352</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C298" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D298" s="0" t="n">
         <v>2017</v>
@@ -3701,20 +4488,20 @@
         <v>4</v>
       </c>
       <c r="D299" s="0" t="s">
-        <v>296</v>
+        <v>353</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C300" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D300" s="0" t="s">
-        <v>297</v>
+        <v>354</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C301" s="0" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D301" s="0" t="n">
         <v>2009</v>
@@ -3722,7 +4509,7 @@
     </row>
     <row r="302" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="C302" s="0" t="s">
         <v>17</v>
@@ -3730,15 +4517,15 @@
     </row>
     <row r="303" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C303" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D303" s="0" t="s">
-        <v>298</v>
+        <v>355</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C304" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D304" s="0" t="n">
         <v>2011</v>
@@ -3746,15 +4533,15 @@
     </row>
     <row r="305" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C305" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D305" s="0" t="s">
-        <v>299</v>
+        <v>356</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C306" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D306" s="0" t="n">
         <v>2008</v>
@@ -3762,15 +4549,15 @@
     </row>
     <row r="307" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C307" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D307" s="0" t="s">
-        <v>300</v>
+        <v>357</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C308" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D308" s="0" t="n">
         <v>2007</v>
@@ -3778,15 +4565,15 @@
     </row>
     <row r="309" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C309" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D309" s="0" t="s">
-        <v>301</v>
+        <v>358</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C310" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D310" s="0" t="n">
         <v>2004</v>
@@ -3794,15 +4581,15 @@
     </row>
     <row r="311" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C311" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>302</v>
+        <v>359</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C312" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D312" s="0" t="n">
         <v>2006</v>
@@ -3810,15 +4597,15 @@
     </row>
     <row r="313" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C313" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>303</v>
+        <v>360</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C314" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D314" s="0" t="n">
         <v>2011</v>
@@ -3826,15 +4613,15 @@
     </row>
     <row r="315" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C315" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D315" s="0" t="s">
-        <v>304</v>
+        <v>361</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C316" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D316" s="0" t="n">
         <v>2013</v>
@@ -3842,15 +4629,15 @@
     </row>
     <row r="317" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C317" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>305</v>
+        <v>362</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C318" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D318" s="0" t="n">
         <v>2011</v>
@@ -3858,15 +4645,15 @@
     </row>
     <row r="319" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C319" s="0" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C320" s="0" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="D320" s="0" t="n">
         <v>2013</v>
@@ -3874,26 +4661,26 @@
     </row>
     <row r="321" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>307</v>
+        <v>364</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="0" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>308</v>
+        <v>365</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="s">
-        <v>170</v>
+        <v>224</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3902,7 +4689,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D26" r:id="rId1" display="https://www.youtube.com/channel/UCPeG-JX2dB90P3RgZbVNheg"/>
-    <hyperlink ref="C323" r:id="rId2" display="https://kpu.go.id/koleksigambar/BB.2_PPWP_1.pdf"/>
+    <hyperlink ref="F130" r:id="rId2" display="https://kpu.go.id/koleksigambar/BB.2_PPWP_2.pdf"/>
+    <hyperlink ref="C323" r:id="rId3" display="https://kpu.go.id/koleksigambar/BB.2_PPWP_1.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3942,22 +4730,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3965,359 +4753,359 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>314</v>
+        <v>371</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>314</v>
+        <v>371</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>316</v>
+        <v>373</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>43</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>47</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>48</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="0" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>52</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>53</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="0" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>57</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>58</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="0" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>52</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>61</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="0" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>57</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>64</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>323</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4350,23 +5138,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>324</v>
+        <v>381</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>325</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>326</v>
+        <v>383</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>327</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>328</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>